<commit_message>
Add logs REST 1000
</commit_message>
<xml_diff>
--- a/test/sorting times.xlsx
+++ b/test/sorting times.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3049301A-967B-4D36-8CFA-D3525E1F018D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF558C4-C662-40E6-8463-25E2AAB97ABB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="32">
   <si>
     <t>GRPC</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>eks 3-3-1</t>
+  </si>
+  <si>
+    <t>REST 3-3-1</t>
   </si>
 </sst>
 </file>
@@ -486,7 +489,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -499,7 +502,7 @@
     <col min="7" max="7" width="25.7109375" customWidth="1"/>
     <col min="8" max="8" width="18.7109375" customWidth="1"/>
     <col min="9" max="9" width="23.140625" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -707,10 +710,10 @@
         <v>161.0818644</v>
       </c>
       <c r="I13" s="8">
-        <v>138.69999999999999</v>
+        <v>138.69764079999999</v>
       </c>
       <c r="J13" s="8">
-        <v>176.93</v>
+        <v>176.93045740000002</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -752,17 +755,29 @@
       <c r="B15" s="1">
         <v>100</v>
       </c>
-      <c r="C15">
-        <v>15.73</v>
-      </c>
-      <c r="D15">
-        <v>13.75</v>
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" t="s">
+        <v>18</v>
       </c>
       <c r="G15">
-        <v>15.73</v>
+        <v>13.750628653488187</v>
       </c>
       <c r="H15">
-        <v>13.75</v>
+        <v>15.730368793215744</v>
+      </c>
+      <c r="I15">
+        <v>4.3084736182900008</v>
+      </c>
+      <c r="J15">
+        <v>6.1620120192100023</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -778,11 +793,23 @@
       <c r="D16" t="s">
         <v>18</v>
       </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" t="s">
+        <v>18</v>
+      </c>
       <c r="G16">
-        <v>43.7</v>
+        <v>37.602944067000003</v>
       </c>
       <c r="H16">
-        <v>37.6</v>
+        <v>43.573344314000003</v>
+      </c>
+      <c r="I16">
+        <v>17.184743181666665</v>
+      </c>
+      <c r="J16">
+        <v>21.656012895</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -812,7 +839,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2849,10 +2876,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1199D7BD-2C02-4FDE-B11D-DB9E8C615E49}">
-  <dimension ref="A1:D640"/>
+  <dimension ref="A1:F640"/>
   <sheetViews>
-    <sheetView topLeftCell="A634" workbookViewId="0">
-      <selection activeCell="C640" sqref="C640:D640"/>
+    <sheetView topLeftCell="A615" workbookViewId="0">
+      <selection activeCell="D640" sqref="D640"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2860,9 +2887,12 @@
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="29.28515625" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -2875,8 +2905,11 @@
       <c r="D1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0.77858455299999996</v>
       </c>
@@ -2889,8 +2922,14 @@
       <c r="D2" s="3">
         <v>6.0140684269999998</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>2.7292020950000002</v>
+      </c>
+      <c r="F2">
+        <v>2.6596028999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1.0811028789999999</v>
       </c>
@@ -2903,8 +2942,14 @@
       <c r="D3" s="3">
         <v>6.1269216220000002</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>2.9139598539999998</v>
+      </c>
+      <c r="F3">
+        <v>2.7710083000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1.0629291400000001</v>
       </c>
@@ -2917,8 +2962,14 @@
       <c r="D4" s="3">
         <v>6.3376646670000003</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>3.1439539270000001</v>
+      </c>
+      <c r="F4">
+        <v>2.4935236999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1.0638224169999999</v>
       </c>
@@ -2931,8 +2982,14 @@
       <c r="D5" s="3">
         <v>6.6952383800000002</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>3.1168107580000002</v>
+      </c>
+      <c r="F5">
+        <v>2.9569702000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1.100458588</v>
       </c>
@@ -2945,8 +3002,14 @@
       <c r="D6" s="3">
         <v>6.8766451139999996</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>3.6095598780000002</v>
+      </c>
+      <c r="F6">
+        <v>2.9653646</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1.1157513999999999</v>
       </c>
@@ -2959,8 +3022,14 @@
       <c r="D7" s="3">
         <v>7.4763626810000003</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>3.5372892679999999</v>
+      </c>
+      <c r="F7">
+        <v>3.1649807999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1.2537087010000001</v>
       </c>
@@ -2973,8 +3042,14 @@
       <c r="D8" s="3">
         <v>6.9736250240000004</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>4.5987032460000004</v>
+      </c>
+      <c r="F8">
+        <v>3.1833494999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1.2511996649999999</v>
       </c>
@@ -2987,8 +3062,14 @@
       <c r="D9" s="3">
         <v>7.4725337319999996</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>4.4964910839999996</v>
+      </c>
+      <c r="F9">
+        <v>3.2757296</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1.2222489990000001</v>
       </c>
@@ -3001,8 +3082,14 @@
       <c r="D10" s="3">
         <v>7.7022594089999998</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>4.8271058739999999</v>
+      </c>
+      <c r="F10">
+        <v>3.8505536</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1.252723426</v>
       </c>
@@ -3015,8 +3102,14 @@
       <c r="D11" s="3">
         <v>7.8289537549999997</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>5.2292365260000002</v>
+      </c>
+      <c r="F11">
+        <v>3.4217824000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1.2474435610000001</v>
       </c>
@@ -3029,8 +3122,14 @@
       <c r="D12" s="3">
         <v>8.1710559259999993</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>5.1695034389999996</v>
+      </c>
+      <c r="F12">
+        <v>3.4980422</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1.2802617270000001</v>
       </c>
@@ -3043,8 +3142,14 @@
       <c r="D13" s="3">
         <v>7.8542407169999997</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>5.5189861010000003</v>
+      </c>
+      <c r="F13">
+        <v>3.5828985000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1.25652633</v>
       </c>
@@ -3057,8 +3162,14 @@
       <c r="D14" s="3">
         <v>8.1063505510000002</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>5.3165870320000002</v>
+      </c>
+      <c r="F14">
+        <v>3.5399067999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1.306316467</v>
       </c>
@@ -3071,8 +3182,14 @@
       <c r="D15" s="3">
         <v>8.1531721459999993</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>5.5389775529999996</v>
+      </c>
+      <c r="F15">
+        <v>3.2353968000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1.280151931</v>
       </c>
@@ -3085,8 +3202,14 @@
       <c r="D16" s="3">
         <v>8.19312811</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>5.4808187220000004</v>
+      </c>
+      <c r="F16">
+        <v>3.5354155</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1.2866465659999999</v>
       </c>
@@ -3099,8 +3222,14 @@
       <c r="D17" s="3">
         <v>8.2186537600000005</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>5.4470838060000002</v>
+      </c>
+      <c r="F17">
+        <v>3.1915398000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1.3535559690000001</v>
       </c>
@@ -3113,8 +3242,14 @@
       <c r="D18" s="3">
         <v>8.4448828989999996</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>5.585373594</v>
+      </c>
+      <c r="F18">
+        <v>3.3686238999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1.3308015449999999</v>
       </c>
@@ -3127,8 +3262,14 @@
       <c r="D19" s="3">
         <v>8.4530947869999995</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>5.3054562809999997</v>
+      </c>
+      <c r="F19">
+        <v>3.5266548000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1.326635252</v>
       </c>
@@ -3141,8 +3282,14 @@
       <c r="D20" s="3">
         <v>8.3832109950000007</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>5.4838470340000001</v>
+      </c>
+      <c r="F20">
+        <v>3.4087679</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1.333289583</v>
       </c>
@@ -3155,8 +3302,14 @@
       <c r="D21" s="3">
         <v>8.9698316479999995</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>5.3643920979999997</v>
+      </c>
+      <c r="F21">
+        <v>3.4928642000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1.3366926960000001</v>
       </c>
@@ -3169,8 +3322,14 @@
       <c r="D22" s="3">
         <v>8.6166519729999997</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>5.564598814</v>
+      </c>
+      <c r="F22">
+        <v>3.8123749</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1.340300405</v>
       </c>
@@ -3183,8 +3342,14 @@
       <c r="D23" s="3">
         <v>9.2700602589999992</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <v>5.576904334</v>
+      </c>
+      <c r="F23">
+        <v>4.1859776999999996</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1.3395686229999999</v>
       </c>
@@ -3197,8 +3362,14 @@
       <c r="D24" s="3">
         <v>8.8779855459999997</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <v>5.8230850920000004</v>
+      </c>
+      <c r="F24">
+        <v>3.2420076</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1.3628506330000001</v>
       </c>
@@ -3211,8 +3382,14 @@
       <c r="D25" s="3">
         <v>8.8314831419999997</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <v>5.7911737499999996</v>
+      </c>
+      <c r="F25">
+        <v>3.9184050099999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1.3706620350000001</v>
       </c>
@@ -3225,8 +3402,14 @@
       <c r="D26" s="3">
         <v>9.2757160219999992</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <v>6.0380679900000001</v>
+      </c>
+      <c r="F26">
+        <v>4.10686252</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1.328902094</v>
       </c>
@@ -3239,8 +3422,14 @@
       <c r="D27" s="3">
         <v>10.019014104</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <v>6.0833704510000004</v>
+      </c>
+      <c r="F27">
+        <v>3.6357332000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1.3512097279999999</v>
       </c>
@@ -3253,8 +3442,14 @@
       <c r="D28" s="3">
         <v>10.289918551</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <v>5.8982805999999997</v>
+      </c>
+      <c r="F28">
+        <v>3.6813950520000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1.3582133510000001</v>
       </c>
@@ -3267,8 +3462,14 @@
       <c r="D29" s="3">
         <v>10.399235063000001</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <v>5.9941151819999998</v>
+      </c>
+      <c r="F29">
+        <v>4.6583094000000003</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1.3598977080000001</v>
       </c>
@@ -3281,8 +3482,14 @@
       <c r="D30" s="3">
         <v>10.076922261</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <v>6.0378043789999998</v>
+      </c>
+      <c r="F30">
+        <v>3.3637171000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1.374568236</v>
       </c>
@@ -3295,8 +3502,14 @@
       <c r="D31" s="3">
         <v>9.9485328309999996</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <v>6.1409867250000003</v>
+      </c>
+      <c r="F31">
+        <v>3.9316867000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1.3531775779999999</v>
       </c>
@@ -3309,8 +3522,14 @@
       <c r="D32" s="3">
         <v>9.9498184240000001</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <v>6.1179224650000004</v>
+      </c>
+      <c r="F32">
+        <v>3.4166753999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1.38938026</v>
       </c>
@@ -3323,8 +3542,14 @@
       <c r="D33" s="3">
         <v>10.240484793</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <v>6.2360980110000002</v>
+      </c>
+      <c r="F33">
+        <v>3.4902481999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1.3608262849999999</v>
       </c>
@@ -3337,8 +3562,14 @@
       <c r="D34" s="3">
         <v>10.564203115</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <v>5.8665021900000003</v>
+      </c>
+      <c r="F34">
+        <v>3.5571111800000002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1.414408025</v>
       </c>
@@ -3351,8 +3582,14 @@
       <c r="D35" s="3">
         <v>10.348661608</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <v>6.2284837020000001</v>
+      </c>
+      <c r="F35">
+        <v>4.8283408000000003</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1.3960752910000001</v>
       </c>
@@ -3365,8 +3602,14 @@
       <c r="D36" s="3">
         <v>10.244604933</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <v>6.3322860570000001</v>
+      </c>
+      <c r="F36">
+        <v>3.6437355999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1.411738793</v>
       </c>
@@ -3379,8 +3622,14 @@
       <c r="D37" s="3">
         <v>10.663485267</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <v>6.2266006489999999</v>
+      </c>
+      <c r="F37">
+        <v>3.7052955000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1.4049432660000001</v>
       </c>
@@ -3393,8 +3642,14 @@
       <c r="D38" s="3">
         <v>10.402719613</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <v>6.560785804</v>
+      </c>
+      <c r="F38">
+        <v>3.9050850000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1.42010098</v>
       </c>
@@ -3407,8 +3662,14 @@
       <c r="D39" s="3">
         <v>10.483664729999999</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39">
+        <v>6.2869866639999996</v>
+      </c>
+      <c r="F39">
+        <v>4.6746353000000003</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1.4367728580000001</v>
       </c>
@@ -3421,8 +3682,14 @@
       <c r="D40" s="3">
         <v>10.654129826</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40">
+        <v>6.212184014</v>
+      </c>
+      <c r="F40">
+        <v>3.9259944</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1.413953536</v>
       </c>
@@ -3435,8 +3702,14 @@
       <c r="D41" s="3">
         <v>10.877011887</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41">
+        <v>6.519280416</v>
+      </c>
+      <c r="F41">
+        <v>4.8478918000000002</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1.4001005879999999</v>
       </c>
@@ -3449,8 +3722,14 @@
       <c r="D42" s="3">
         <v>11.315302622000001</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42">
+        <v>6.4699012099999997</v>
+      </c>
+      <c r="F42">
+        <v>4.1798651199999997</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1.4372518460000001</v>
       </c>
@@ -3463,8 +3742,14 @@
       <c r="D43" s="3">
         <v>11.596810618999999</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43">
+        <v>6.1531579550000002</v>
+      </c>
+      <c r="F43">
+        <v>4.3754077999999996</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1.405866442</v>
       </c>
@@ -3477,8 +3762,14 @@
       <c r="D44" s="3">
         <v>10.968086604</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44">
+        <v>6.3862713260000001</v>
+      </c>
+      <c r="F44">
+        <v>4.7767412</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1.4311913000000001</v>
       </c>
@@ -3491,8 +3782,14 @@
       <c r="D45" s="3">
         <v>11.13148097</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45">
+        <v>6.2192567480000003</v>
+      </c>
+      <c r="F45">
+        <v>3.8506687999999998</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1.4111225080000001</v>
       </c>
@@ -3505,8 +3802,14 @@
       <c r="D46" s="3">
         <v>10.990204818</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46">
+        <v>6.2869239700000001</v>
+      </c>
+      <c r="F46">
+        <v>4.5060402599999998</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>1.4142357290000001</v>
       </c>
@@ -3519,8 +3822,14 @@
       <c r="D47" s="3">
         <v>11.046846974999999</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47">
+        <v>6.5656919519999999</v>
+      </c>
+      <c r="F47">
+        <v>4.4578930000000003</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1.4349836039999999</v>
       </c>
@@ -3533,8 +3842,14 @@
       <c r="D48" s="3">
         <v>11.070333354000001</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48">
+        <v>6.2167255969999999</v>
+      </c>
+      <c r="F48">
+        <v>4.0761202000000001</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>1.452897149</v>
       </c>
@@ -3547,8 +3862,14 @@
       <c r="D49" s="3">
         <v>11.075460442000001</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49">
+        <v>6.4600795460000002</v>
+      </c>
+      <c r="F49">
+        <v>3.3852497000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>1.477455926</v>
       </c>
@@ -3561,8 +3882,14 @@
       <c r="D50" s="3">
         <v>11.144902159000001</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50">
+        <v>6.473771878</v>
+      </c>
+      <c r="F50">
+        <v>3.9930544000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>1.466490904</v>
       </c>
@@ -3575,8 +3902,14 @@
       <c r="D51" s="3">
         <v>11.117522962000001</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51">
+        <v>6.6505234980000001</v>
+      </c>
+      <c r="F51">
+        <v>3.9562780000000002</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>1.4477659789999999</v>
       </c>
@@ -3589,8 +3922,14 @@
       <c r="D52" s="3">
         <v>11.139934684</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52">
+        <v>6.6377352509999996</v>
+      </c>
+      <c r="F52">
+        <v>4.4237745000000004</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>1.475075787</v>
       </c>
@@ -3603,8 +3942,14 @@
       <c r="D53" s="3">
         <v>10.868018545</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53">
+        <v>6.3115777800000004</v>
+      </c>
+      <c r="F53">
+        <v>4.4766726099999996</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>1.496265449</v>
       </c>
@@ -3617,8 +3962,14 @@
       <c r="D54" s="3">
         <v>11.184904305</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54">
+        <v>6.3890873160000003</v>
+      </c>
+      <c r="F54">
+        <v>3.9798605</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>1.4753924780000001</v>
       </c>
@@ -3631,8 +3982,14 @@
       <c r="D55" s="3">
         <v>11.171271378</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E55">
+        <v>6.2415698959999997</v>
+      </c>
+      <c r="F55">
+        <v>3.9136272999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>1.449786228</v>
       </c>
@@ -3645,8 +4002,14 @@
       <c r="D56" s="3">
         <v>11.309250034</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56">
+        <v>6.2071788630000002</v>
+      </c>
+      <c r="F56">
+        <v>3.6371042</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>1.4767615439999999</v>
       </c>
@@ -3659,8 +4022,14 @@
       <c r="D57" s="3">
         <v>11.836908258999999</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57">
+        <v>6.6794662809999998</v>
+      </c>
+      <c r="F57">
+        <v>5.3780419000000004</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>1.4754027780000001</v>
       </c>
@@ -3673,8 +4042,14 @@
       <c r="D58" s="3">
         <v>11.234538068000001</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58">
+        <v>6.7095222310000002</v>
+      </c>
+      <c r="F58">
+        <v>4.4100102000000003</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>1.4787494940000001</v>
       </c>
@@ -3687,8 +4062,14 @@
       <c r="D59" s="3">
         <v>11.359813834000001</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59">
+        <v>6.7302938220000001</v>
+      </c>
+      <c r="F59">
+        <v>4.6377058</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>1.4648238469999999</v>
       </c>
@@ -3701,8 +4082,14 @@
       <c r="D60" s="3">
         <v>11.339555472000001</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60">
+        <v>6.6177953819999997</v>
+      </c>
+      <c r="F60">
+        <v>5.3390423</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>1.4897063150000001</v>
       </c>
@@ -3715,8 +4102,14 @@
       <c r="D61" s="3">
         <v>12.180681012000001</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61">
+        <v>6.4228901389999997</v>
+      </c>
+      <c r="F61">
+        <v>4.6269254999999996</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>1.5000034550000001</v>
       </c>
@@ -3729,8 +4122,14 @@
       <c r="D62" s="3">
         <v>11.442001775</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E62">
+        <v>6.6581084649999998</v>
+      </c>
+      <c r="F62">
+        <v>4.0187423000000004</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>1.5037746590000001</v>
       </c>
@@ -3743,8 +4142,14 @@
       <c r="D63" s="3">
         <v>11.919650086000001</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E63">
+        <v>6.7782667529999996</v>
+      </c>
+      <c r="F63">
+        <v>4.3591581000000001</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>1.530062392</v>
       </c>
@@ -3757,8 +4162,14 @@
       <c r="D64" s="3">
         <v>12.194202659</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64">
+        <v>6.6298860089999998</v>
+      </c>
+      <c r="F64">
+        <v>5.3143018</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>1.5245235319999999</v>
       </c>
@@ -3771,8 +4182,14 @@
       <c r="D65" s="3">
         <v>12.302826897999999</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65">
+        <v>6.4391638999999996</v>
+      </c>
+      <c r="F65">
+        <v>4.2059369770000004</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>1.5138236030000001</v>
       </c>
@@ -3785,8 +4202,14 @@
       <c r="D66" s="3">
         <v>11.506742687999999</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66">
+        <v>6.8219661360000003</v>
+      </c>
+      <c r="F66">
+        <v>4.5312963999999996</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>1.5279821440000001</v>
       </c>
@@ -3799,8 +4222,14 @@
       <c r="D67" s="3">
         <v>11.800582126</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67">
+        <v>6.697374194</v>
+      </c>
+      <c r="F67">
+        <v>5.3757216999999997</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>1.5139233009999999</v>
       </c>
@@ -3813,8 +4242,14 @@
       <c r="D68" s="3">
         <v>11.81700098</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E68">
+        <v>6.7323871659999996</v>
+      </c>
+      <c r="F68">
+        <v>5.1588295999999998</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>1.5385575760000001</v>
       </c>
@@ -3827,8 +4262,14 @@
       <c r="D69" s="3">
         <v>12.368820381999999</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E69">
+        <v>6.8254081480000002</v>
+      </c>
+      <c r="F69">
+        <v>4.8623154</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>1.5000195540000001</v>
       </c>
@@ -3841,8 +4282,14 @@
       <c r="D70" s="3">
         <v>13.061856619</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E70">
+        <v>6.8129000839999998</v>
+      </c>
+      <c r="F70">
+        <v>4.9291479000000002</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>1.536555728</v>
       </c>
@@ -3855,8 +4302,14 @@
       <c r="D71" s="3">
         <v>12.57347818</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E71">
+        <v>6.6607811410000002</v>
+      </c>
+      <c r="F71">
+        <v>4.3111549</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>1.5066333860000001</v>
       </c>
@@ -3869,8 +4322,14 @@
       <c r="D72" s="3">
         <v>12.594589686000001</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E72">
+        <v>6.7392139579999997</v>
+      </c>
+      <c r="F72">
+        <v>5.1220546000000002</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>1.528771925</v>
       </c>
@@ -3883,8 +4342,14 @@
       <c r="D73" s="3">
         <v>12.387751759</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E73">
+        <v>6.6252405019999996</v>
+      </c>
+      <c r="F73">
+        <v>5.3133235000000001</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>1.516089646</v>
       </c>
@@ -3897,8 +4362,14 @@
       <c r="D74" s="3">
         <v>12.970843278</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E74">
+        <v>6.7809710550000002</v>
+      </c>
+      <c r="F74">
+        <v>4.6966323000000001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>1.557985484</v>
       </c>
@@ -3911,8 +4382,14 @@
       <c r="D75" s="3">
         <v>13.066520601000001</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E75">
+        <v>6.8740536219999999</v>
+      </c>
+      <c r="F75">
+        <v>5.2325647999999996</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>1.5262221890000001</v>
       </c>
@@ -3925,8 +4402,14 @@
       <c r="D76" s="3">
         <v>13.07005204</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E76">
+        <v>6.8191149170000003</v>
+      </c>
+      <c r="F76">
+        <v>4.1134607000000001</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>1.5289672190000001</v>
       </c>
@@ -3939,8 +4422,14 @@
       <c r="D77" s="3">
         <v>12.401334018</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E77">
+        <v>6.9005769050000003</v>
+      </c>
+      <c r="F77">
+        <v>5.5676473</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>1.5595761429999999</v>
       </c>
@@ -3953,8 +4442,14 @@
       <c r="D78" s="3">
         <v>12.654588299</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E78">
+        <v>6.996686167</v>
+      </c>
+      <c r="F78">
+        <v>4.9003757999999999</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>1.5379200930000001</v>
       </c>
@@ -3967,8 +4462,14 @@
       <c r="D79" s="3">
         <v>13.493122058000001</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E79">
+        <v>6.7046614670000002</v>
+      </c>
+      <c r="F79">
+        <v>5.1176437999999997</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>1.548700819</v>
       </c>
@@ -3981,8 +4482,14 @@
       <c r="D80" s="3">
         <v>12.404834855000001</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E80">
+        <v>6.8529256419999998</v>
+      </c>
+      <c r="F80">
+        <v>5.1366923</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>1.593832374</v>
       </c>
@@ -3995,8 +4502,14 @@
       <c r="D81" s="3">
         <v>13.07752271</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E81">
+        <v>6.9999965639999999</v>
+      </c>
+      <c r="F81">
+        <v>5.1673888000000003</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>1.557241103</v>
       </c>
@@ -4009,8 +4522,14 @@
       <c r="D82" s="3">
         <v>12.727151655</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E82">
+        <v>6.9669746080000001</v>
+      </c>
+      <c r="F82">
+        <v>5.4927469999999996</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>1.581739681</v>
       </c>
@@ -4023,8 +4542,14 @@
       <c r="D83" s="3">
         <v>12.717983714000001</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E83">
+        <v>6.655363973</v>
+      </c>
+      <c r="F83">
+        <v>5.0173715999999997</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>1.593429585</v>
       </c>
@@ -4037,8 +4562,14 @@
       <c r="D84" s="3">
         <v>13.228700440000001</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E84">
+        <v>7.0528115800000002</v>
+      </c>
+      <c r="F84">
+        <v>4.9957159000000004</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>1.6216530689999999</v>
       </c>
@@ -4051,8 +4582,14 @@
       <c r="D85" s="3">
         <v>12.442001448999999</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E85">
+        <v>6.7012618760000002</v>
+      </c>
+      <c r="F85">
+        <v>4.4617491999999999</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>1.622232954</v>
       </c>
@@ -4065,8 +4602,14 @@
       <c r="D86" s="3">
         <v>12.829662197999999</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E86">
+        <v>6.8289866049999999</v>
+      </c>
+      <c r="F86">
+        <v>5.3272054000000004</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>1.631696614</v>
       </c>
@@ -4079,8 +4622,14 @@
       <c r="D87" s="3">
         <v>11.964599323</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E87">
+        <v>6.7347660549999997</v>
+      </c>
+      <c r="F87">
+        <v>5.2625881999999997</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>1.6118298170000001</v>
       </c>
@@ -4093,8 +4642,14 @@
       <c r="D88" s="3">
         <v>12.939983403999999</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E88">
+        <v>6.8580385939999999</v>
+      </c>
+      <c r="F88">
+        <v>5.3740496000000002</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>1.5951107419999999</v>
       </c>
@@ -4107,8 +4662,14 @@
       <c r="D89" s="3">
         <v>12.906188711</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E89">
+        <v>6.8045120710000004</v>
+      </c>
+      <c r="F89">
+        <v>4.9401090999999999</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>1.650528336</v>
       </c>
@@ -4121,8 +4682,14 @@
       <c r="D90" s="3">
         <v>13.688396022999999</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E90">
+        <v>6.9116560070000004</v>
+      </c>
+      <c r="F90">
+        <v>5.1381157000000002</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>1.649128672</v>
       </c>
@@ -4135,8 +4702,14 @@
       <c r="D91" s="3">
         <v>12.555652064</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E91">
+        <v>6.867791134</v>
+      </c>
+      <c r="F91">
+        <v>4.6208998000000001</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>1.6362815980000001</v>
       </c>
@@ -4149,8 +4722,14 @@
       <c r="D92" s="3">
         <v>12.897988127</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E92">
+        <v>6.834486751</v>
+      </c>
+      <c r="F92">
+        <v>4.8576239000000001</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>1.640531389</v>
       </c>
@@ -4163,8 +4742,14 @@
       <c r="D93" s="3">
         <v>14.276693885</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E93">
+        <v>6.9510964380000004</v>
+      </c>
+      <c r="F93">
+        <v>5.3338840000000003</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>1.6193989259999999</v>
       </c>
@@ -4177,8 +4762,14 @@
       <c r="D94" s="3">
         <v>13.617615244</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E94">
+        <v>6.8751466639999999</v>
+      </c>
+      <c r="F94">
+        <v>5.1581833000000001</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>1.663799899</v>
       </c>
@@ -4191,8 +4782,14 @@
       <c r="D95" s="3">
         <v>13.372976915000001</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E95">
+        <v>7.0154446520000002</v>
+      </c>
+      <c r="F95">
+        <v>5.3624752000000004</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>1.623730216</v>
       </c>
@@ -4205,8 +4802,14 @@
       <c r="D96" s="3">
         <v>13.75075745</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E96">
+        <v>6.9260482249999997</v>
+      </c>
+      <c r="F96">
+        <v>5.2062884</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>1.6584074360000001</v>
       </c>
@@ -4219,8 +4822,14 @@
       <c r="D97" s="3">
         <v>14.439011784</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E97">
+        <v>7.1113083750000001</v>
+      </c>
+      <c r="F97">
+        <v>4.7772959999999998</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>1.66967555</v>
       </c>
@@ -4233,8 +4842,14 @@
       <c r="D98" s="3">
         <v>14.207832</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E98">
+        <v>6.8360576020000003</v>
+      </c>
+      <c r="F98">
+        <v>5.0907201999999998</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>1.676644574</v>
       </c>
@@ -4247,8 +4862,14 @@
       <c r="D99" s="3">
         <v>13.609579981</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E99">
+        <v>7.0772938749999996</v>
+      </c>
+      <c r="F99">
+        <v>5.8177897999999999</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>1.674032741</v>
       </c>
@@ -4261,8 +4882,14 @@
       <c r="D100" s="3">
         <v>15.048310373</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E100">
+        <v>6.8878230739999999</v>
+      </c>
+      <c r="F100">
+        <v>5.3739559000000003</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>1.644133399</v>
       </c>
@@ -4275,8 +4902,14 @@
       <c r="D101" s="3">
         <v>5.8179467799999998</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E101">
+        <v>7.1763748669999998</v>
+      </c>
+      <c r="F101">
+        <v>5.7696630000000004</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C102" s="3">
         <v>15.9700004</v>
       </c>
@@ -4284,7 +4917,7 @@
         <v>15.732971581999999</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103">
         <f>AVERAGE(A2:A101)</f>
         <v>1.4398487849800004</v>
@@ -4299,8 +4932,16 @@
       <c r="D103" s="3">
         <v>5.8663770770000001</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E103">
+        <f>AVERAGE(E2:E101)</f>
+        <v>6.1620120192100023</v>
+      </c>
+      <c r="F103">
+        <f>AVERAGE(F2:F101)</f>
+        <v>4.3084736182900008</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C104" s="3">
         <v>5.7890237820000001</v>
       </c>
@@ -4308,7 +4949,7 @@
         <v>5.6713183110000003</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C105" s="3">
         <v>5.6255030149999996</v>
       </c>
@@ -4316,7 +4957,7 @@
         <v>5.5441266560000004</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C106" s="3">
         <v>6.0765470820000003</v>
       </c>
@@ -4324,7 +4965,7 @@
         <v>5.9912315209999996</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C107" s="3">
         <v>7.3595656969999999</v>
       </c>
@@ -4332,7 +4973,7 @@
         <v>7.3074566599999997</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C108" s="3">
         <v>7.3231612149999998</v>
       </c>
@@ -4340,7 +4981,7 @@
         <v>7.2759916049999998</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C109" s="3">
         <v>8.0344063820000002</v>
       </c>
@@ -4348,7 +4989,7 @@
         <v>7.992925982</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C110" s="3">
         <v>8.5644217190000003</v>
       </c>
@@ -4356,7 +4997,7 @@
         <v>8.5215931430000005</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C111" s="3">
         <v>8.6182543250000005</v>
       </c>
@@ -4364,7 +5005,7 @@
         <v>8.5772299010000008</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C112" s="3">
         <v>8.8793587049999996</v>
       </c>
@@ -8589,10 +9230,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A8061C1-9648-4EFA-A3A4-168D1121A1B2}">
-  <dimension ref="A1:D139"/>
+  <dimension ref="A1:F139"/>
   <sheetViews>
-    <sheetView topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="D91" sqref="D91"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8601,9 +9242,11 @@
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
     <col min="3" max="3" width="20.5703125" customWidth="1"/>
     <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -8616,8 +9259,11 @@
       <c r="D1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>0.92324879699999995</v>
       </c>
@@ -8630,8 +9276,14 @@
       <c r="D2" s="3">
         <v>0.77393198399999996</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>20.492216899999999</v>
+      </c>
+      <c r="F2">
+        <v>16.025558499999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1.029589517</v>
       </c>
@@ -8644,8 +9296,14 @@
       <c r="D3" s="3">
         <v>0.82183431900000004</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>21.34514136</v>
+      </c>
+      <c r="F3">
+        <v>16.244249799999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>1.281601502</v>
       </c>
@@ -8658,8 +9316,14 @@
       <c r="D4" s="3">
         <v>0.79898597400000004</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>21.37176861</v>
+      </c>
+      <c r="F4">
+        <v>15.7957144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>1.282543379</v>
       </c>
@@ -8672,8 +9336,14 @@
       <c r="D5" s="3">
         <v>0.87100302399999996</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>21.800629149999999</v>
+      </c>
+      <c r="F5">
+        <v>20.504618700000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>1.2316617139999999</v>
       </c>
@@ -8686,8 +9356,14 @@
       <c r="D6" s="3">
         <v>0.85812303700000003</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>22.26721723</v>
+      </c>
+      <c r="F6">
+        <v>17.2695373</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>1.5337634840000001</v>
       </c>
@@ -8700,8 +9376,14 @@
       <c r="D7" s="3">
         <v>1.0756456489999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>22.659104119999999</v>
+      </c>
+      <c r="F7">
+        <v>17.26878039</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>1.738468616</v>
       </c>
@@ -8715,7 +9397,7 @@
         <v>1.172763987</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>1.8397801579999999</v>
       </c>
@@ -8728,8 +9410,16 @@
       <c r="D9" s="3">
         <v>1.1845107020000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <f>AVERAGE(E2:E7)</f>
+        <v>21.656012895</v>
+      </c>
+      <c r="F9">
+        <f>AVERAGE(F2:F7)</f>
+        <v>17.184743181666665</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>2.060125212</v>
       </c>
@@ -8743,7 +9433,7 @@
         <v>1.3795542599999999</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>2.1087661309999999</v>
       </c>
@@ -8757,7 +9447,7 @@
         <v>1.352761112</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>2.293480749</v>
       </c>
@@ -8771,7 +9461,7 @@
         <v>1.4613417719999999</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>2.3970103370000002</v>
       </c>
@@ -8785,7 +9475,7 @@
         <v>1.3876998620000001</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>2.4185489150000001</v>
       </c>
@@ -8799,7 +9489,7 @@
         <v>1.3814995130000001</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>2.5231751770000002</v>
       </c>
@@ -8813,7 +9503,7 @@
         <v>1.385167724</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>2.5287211420000002</v>
       </c>

</xml_diff>